<commit_message>
Performence and soupUI tests has been added
</commit_message>
<xml_diff>
--- a/manual testing/TaskList-KrishnaVeni.xlsx
+++ b/manual testing/TaskList-KrishnaVeni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mvpstudio-advanceProject\mvpstudio-advance\manual testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F2D062-18EB-4530-B25A-908415BA90A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170CDFD-D494-4702-B1BE-9AEB3CC6C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Test Analyst Name:</t>
   </si>
@@ -108,12 +108,30 @@
   <si>
     <t>Krishna Veni</t>
   </si>
+  <si>
+    <t>https://dog.ceo/api/breeds/list/all</t>
+  </si>
+  <si>
+    <t>SoapUI</t>
+  </si>
+  <si>
+    <t>http://webservices.oorsprong.org/websamples.countryinfo/CountryInfoService.wso?WSDL</t>
+  </si>
+  <si>
+    <t>http://webservices.daehosting.com/services/isbnservice.wso?WSDL</t>
+  </si>
+  <si>
+    <t>Language add, Edit, Get and Delete</t>
+  </si>
+  <si>
+    <t>Data drive through CSV config file, Assertion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -147,17 +165,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -212,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -221,8 +228,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,16 +446,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1014"/>
+  <dimension ref="A1:Z1013"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
@@ -609,7 +614,7 @@
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1"/>
@@ -640,7 +645,7 @@
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="1"/>
@@ -671,7 +676,7 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
@@ -702,7 +707,7 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1"/>
@@ -733,7 +738,7 @@
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="1"/>
@@ -764,7 +769,7 @@
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="1"/>
@@ -795,7 +800,7 @@
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="1"/>
@@ -882,7 +887,7 @@
       <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1"/>
@@ -913,7 +918,7 @@
       <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="1"/>
@@ -944,7 +949,7 @@
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="1"/>
@@ -975,7 +980,7 @@
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="1"/>
@@ -1006,7 +1011,7 @@
       <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="1"/>
@@ -1092,7 +1097,7 @@
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="1"/>
@@ -1123,7 +1128,7 @@
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="1"/>
@@ -1154,7 +1159,7 @@
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="1"/>
@@ -1185,7 +1190,7 @@
       <c r="B25" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="1"/>
@@ -1216,7 +1221,7 @@
       <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="1"/>
@@ -1332,9 +1337,15 @@
     </row>
     <row r="30" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1469,11 +1480,17 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="6"/>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1500,12 +1517,12 @@
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="1"/>
@@ -1534,12 +1551,12 @@
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="1"/>
@@ -1567,7 +1584,15 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="D38" s="9"/>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1591,9 +1616,17 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="D39" s="9"/>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1619,6 +1652,9 @@
     </row>
     <row r="40" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -28886,37 +28922,9 @@
       <c r="Y1013" s="1"/>
       <c r="Z1013" s="1"/>
     </row>
-    <row r="1014" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1014" s="1"/>
-      <c r="B1014" s="1"/>
-      <c r="C1014" s="1"/>
-      <c r="D1014" s="1"/>
-      <c r="E1014" s="1"/>
-      <c r="F1014" s="1"/>
-      <c r="G1014" s="1"/>
-      <c r="H1014" s="1"/>
-      <c r="I1014" s="1"/>
-      <c r="J1014" s="1"/>
-      <c r="K1014" s="1"/>
-      <c r="L1014" s="1"/>
-      <c r="M1014" s="1"/>
-      <c r="N1014" s="1"/>
-      <c r="O1014" s="1"/>
-      <c r="P1014" s="1"/>
-      <c r="Q1014" s="1"/>
-      <c r="R1014" s="1"/>
-      <c r="S1014" s="1"/>
-      <c r="T1014" s="1"/>
-      <c r="U1014" s="1"/>
-      <c r="V1014" s="1"/>
-      <c r="W1014" s="1"/>
-      <c r="X1014" s="1"/>
-      <c r="Y1014" s="1"/>
-      <c r="Z1014" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D22:D26 D6:D11 D15:D19 D29:D32 D35" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D22:D26 D6:D11 D15:D19 D29:D32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Not Yet assigned,In-Progress,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Nunit, specflow and API tests changes has been added
</commit_message>
<xml_diff>
--- a/manual testing/TaskList-KrishnaVeni.xlsx
+++ b/manual testing/TaskList-KrishnaVeni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mvpstudio-advanceProject\mvpstudio-advance\manual testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170CDFD-D494-4702-B1BE-9AEB3CC6C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1145B9-7828-4D15-ACB8-5DDA614202FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Test Analyst Name:</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Data drive through CSV config file, Assertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSTMAN  Data driven </t>
   </si>
 </sst>
 </file>
@@ -448,8 +451,8 @@
   </sheetPr>
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1520,7 +1523,7 @@
         <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>26</v>

</xml_diff>